<commit_message>
Change font name to Khmer Moul Light
</commit_message>
<xml_diff>
--- a/01-Requirement/Score/2-List score for student by semester.xlsx
+++ b/01-Requirement/Score/2-List score for student by semester.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp\vhosts\ume-system\01-Requirement\Score\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="15255" windowHeight="7935" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="15255" windowHeight="7935" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Management" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
     <sheet name="English " sheetId="6" r:id="rId7"/>
     <sheet name="Total Semester" sheetId="2" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -26,7 +31,7 @@
     <author>Sokchea Seang</author>
   </authors>
   <commentList>
-    <comment ref="B35" authorId="0">
+    <comment ref="B35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B91" authorId="0">
+    <comment ref="B91" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +89,7 @@
     <author>Sokchea Seang</author>
   </authors>
   <commentList>
-    <comment ref="B35" authorId="0">
+    <comment ref="B35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -108,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B91" authorId="0">
+    <comment ref="B91" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +147,7 @@
     <author>Sokchea Seang</author>
   </authors>
   <commentList>
-    <comment ref="B35" authorId="0">
+    <comment ref="B35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B40" authorId="0">
+    <comment ref="B40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -190,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B55" authorId="0">
+    <comment ref="B55" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -214,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B91" authorId="0">
+    <comment ref="B91" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -248,7 +253,7 @@
     <author>Sokchea Seang</author>
   </authors>
   <commentList>
-    <comment ref="B35" authorId="0">
+    <comment ref="B35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -272,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B40" authorId="0">
+    <comment ref="B40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -296,7 +301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B55" authorId="0">
+    <comment ref="B55" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -320,7 +325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B91" authorId="0">
+    <comment ref="B91" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -354,7 +359,7 @@
     <author>Sokchea Seang</author>
   </authors>
   <commentList>
-    <comment ref="B35" authorId="0">
+    <comment ref="B35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -378,7 +383,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B40" authorId="0">
+    <comment ref="B40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -402,7 +407,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B55" authorId="0">
+    <comment ref="B55" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -426,7 +431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B91" authorId="0">
+    <comment ref="B91" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -460,7 +465,7 @@
     <author>Sokchea Seang</author>
   </authors>
   <commentList>
-    <comment ref="B35" authorId="0">
+    <comment ref="B35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -484,7 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B40" authorId="0">
+    <comment ref="B40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -508,7 +513,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B55" authorId="0">
+    <comment ref="B55" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -532,7 +537,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B91" authorId="0">
+    <comment ref="B91" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -566,7 +571,7 @@
     <author>Sokchea Seang</author>
   </authors>
   <commentList>
-    <comment ref="B35" authorId="0">
+    <comment ref="B35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -590,7 +595,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B91" authorId="0">
+    <comment ref="B91" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -624,7 +629,7 @@
     <author>Sokchea Seang</author>
   </authors>
   <commentList>
-    <comment ref="B31" authorId="0">
+    <comment ref="B31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -648,7 +653,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B87" authorId="0">
+    <comment ref="B87" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1746,6 +1751,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -6030,15 +6038,15 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="km-KH" sz="1100" u="sng">
-              <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t>ប្រឡងបញ្ចប់មុខវិជ្ជា </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="km-KH" sz="1100" u="sng" baseline="0">
-              <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t>ឆ្នាំមូលដ្ឋាន ជំនាន់ទី១២</a:t>
           </a:r>
@@ -6047,35 +6055,35 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="km-KH" sz="1100" baseline="0">
-              <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t>សិក្សាពេលៈ សៅរ៌-អាទិត្យ បន្ទប់ៈ </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t>C</a:t>
           </a:r>
           <a:endParaRPr lang="km-KH" sz="1100" b="1" baseline="0">
-            <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-            <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+            <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+            <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="km-KH" sz="1100" baseline="0">
-              <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t>ឆ្នាំសិក្សាៈ ២០១៣-២០១៤</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100">
-            <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-            <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+            <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+            <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -6134,15 +6142,15 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="km-KH" sz="1100">
-              <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t>សាកលវិទ្យាល័យគ្រប់គ្រង</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="km-KH" sz="1100" baseline="0">
-              <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t> និងសេដ្ឋកិច្ច </a:t>
           </a:r>
@@ -6151,8 +6159,8 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="km-KH" sz="1100" baseline="0">
-              <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t>ខេត្តកំពង់ចាម</a:t>
           </a:r>
@@ -6220,8 +6228,8 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="km-KH" sz="1100">
-              <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t>ព្រះរាជាណាចក្រកម្ពុជា</a:t>
           </a:r>
@@ -6230,8 +6238,8 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="km-KH" sz="1100" baseline="0">
-              <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t>ជាតិ សាសនា ព្រះមហាក្សត្រ</a:t>
           </a:r>
@@ -6358,9 +6366,9 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="km-KH" sz="1100">
-              <a:latin typeface="Kh Siemreap" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Siemreap" pitchFamily="2" charset="0"/>
+            <a:rPr lang="km-KH" sz="1000">
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t>កំពង់ចាម,ថ្ងៃទី...........ខែ................ឆ្នាំ២០....</a:t>
           </a:r>
@@ -6368,15 +6376,15 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="km-KH" sz="1100">
-              <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+            <a:rPr lang="km-KH" sz="1000">
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t>ប្រធានដេប៉ាតឺម៉ង់ថ្នាក់ឆ្នាំមូលដ្ឋាន</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-            <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+          <a:endParaRPr lang="en-US" sz="1000">
+            <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+            <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -6434,9 +6442,9 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="km-KH" sz="1100">
-              <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+            <a:rPr lang="km-KH" sz="1000">
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t>បានឃើញ និងឯកភាព</a:t>
           </a:r>
@@ -6444,15 +6452,15 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="km-KH" sz="1100">
-              <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-              <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+            <a:rPr lang="km-KH" sz="1000">
+              <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+              <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:t>នាយកសាខា</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:latin typeface="Kh Muol" pitchFamily="2" charset="0"/>
-            <a:cs typeface="Kh Muol" pitchFamily="2" charset="0"/>
+          <a:endParaRPr lang="en-US" sz="1000">
+            <a:latin typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
+            <a:cs typeface="Khmer OS Muol Light" panose="02000500000000020004" pitchFamily="2" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -6505,7 +6513,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6540,7 +6548,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -13254,7 +13262,7 @@
   </sheetPr>
   <dimension ref="A19:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G20" sqref="G20"/>
       <selection pane="bottomLeft" activeCell="I70" sqref="I70"/>
@@ -29855,8 +29863,8 @@
   </sheetPr>
   <dimension ref="A15:P102"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>